<commit_message>
update excel_to_Json_Converter_angularJS add pay load for integration from one instance to other of event dataValue
</commit_message>
<xml_diff>
--- a/Excel to json convertor/sample-format/dataElements_form_name_translations_with_object_property.xlsx
+++ b/Excel to json convertor/sample-format/dataElements_form_name_translations_with_object_property.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitHub_source_code\excel_to_Json_Converter_angularJS\sample-format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC856093-CDD5-4AD2-990A-2C69EF20A9C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B987A7A-ECB9-44F6-95F4-307CF4C8EB92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataElements" sheetId="6" r:id="rId1"/>
@@ -18,12 +18,16 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">dataElements!$D$1:$D$94</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2780" uniqueCount="1052">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2796" uniqueCount="1067">
   <si>
     <t>property</t>
   </si>
@@ -3187,6 +3191,51 @@
   </si>
   <si>
     <t>relationshipTypes</t>
+  </si>
+  <si>
+    <t>my</t>
+  </si>
+  <si>
+    <t>programStages</t>
+  </si>
+  <si>
+    <t>Burmese/Myanmar</t>
+  </si>
+  <si>
+    <t>organisationUnits</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>fr</t>
+  </si>
+  <si>
+    <t>arabic</t>
+  </si>
+  <si>
+    <t>ar</t>
+  </si>
+  <si>
+    <t>Ukrainian (Ukraine)</t>
+  </si>
+  <si>
+    <t>uk_UA</t>
+  </si>
+  <si>
+    <t>dataSets</t>
+  </si>
+  <si>
+    <t>categoryCombos</t>
+  </si>
+  <si>
+    <t>optionSets</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>for trackedEntityAttributes remove form-name then translation work</t>
   </si>
 </sst>
 </file>
@@ -3557,10 +3606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E6B5FAB-DF4A-42DC-8643-A674828EC12D}">
-  <dimension ref="A1:F691"/>
+  <dimension ref="A1:H691"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3570,9 +3619,10 @@
     <col min="4" max="4" width="72.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.90625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -3591,8 +3641,11 @@
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -3611,8 +3664,14 @@
       <c r="F2" s="2" t="s">
         <v>696</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="2" t="s">
+        <v>1054</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -3625,14 +3684,20 @@
       <c r="D3" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>1042</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="2" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -3645,14 +3710,20 @@
       <c r="D4" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>1043</v>
       </c>
       <c r="F4" t="s">
         <v>1044</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>1058</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -3668,8 +3739,14 @@
       <c r="E5" t="s">
         <v>1041</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="2" t="s">
+        <v>1060</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -3686,7 +3763,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -3703,7 +3780,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -3720,7 +3797,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
@@ -3734,10 +3811,10 @@
         <v>358</v>
       </c>
       <c r="E9" t="s">
-        <v>1048</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
@@ -3754,7 +3831,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
@@ -3767,11 +3844,11 @@
       <c r="D11" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="2" t="s">
         <v>1050</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>15</v>
       </c>
@@ -3788,7 +3865,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
@@ -3801,8 +3878,11 @@
       <c r="D13" s="3" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
@@ -3815,8 +3895,11 @@
       <c r="D14" s="4" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>18</v>
       </c>
@@ -3829,8 +3912,11 @@
       <c r="D15" s="4" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>19</v>
       </c>
@@ -3843,8 +3929,11 @@
       <c r="D16" s="3" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>20</v>
       </c>
@@ -3857,8 +3946,11 @@
       <c r="D17" s="3" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
@@ -3872,7 +3964,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>22</v>
       </c>
@@ -3886,7 +3978,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>23</v>
       </c>
@@ -3899,8 +3991,14 @@
       <c r="D20" s="3" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>1065</v>
+      </c>
+      <c r="F20" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>24</v>
       </c>
@@ -3914,7 +4012,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
@@ -3928,7 +4026,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>26</v>
       </c>
@@ -3942,7 +4040,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>27</v>
       </c>
@@ -3956,7 +4054,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>28</v>
       </c>
@@ -3970,7 +4068,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>29</v>
       </c>
@@ -3984,7 +4082,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>30</v>
       </c>
@@ -3998,7 +4096,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>31</v>
       </c>
@@ -4012,7 +4110,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>32</v>
       </c>
@@ -4026,7 +4124,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>33</v>
       </c>
@@ -4040,7 +4138,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>34</v>
       </c>
@@ -4054,7 +4152,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>35</v>
       </c>

</xml_diff>